<commit_message>
change compare GRU and RNN models
</commit_message>
<xml_diff>
--- a/data_origin/DulieuVang,dau,Tygia.xlsx
+++ b/data_origin/DulieuVang,dau,Tygia.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DATN\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DATN\data_origin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C9F25D3-6EDF-4CFE-AAB7-05FFE1C23EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123890F2-3FB0-413B-B097-8C8E1EAC6F67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12257,8 +12257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D868"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A835" workbookViewId="0">
-      <selection activeCell="K861" sqref="K861"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>